<commit_message>
Add colour conversions to fix colours
</commit_message>
<xml_diff>
--- a/protocol/wm_real_0.xlsx
+++ b/protocol/wm_real_0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L\Google Drive\PhD\experiments\adapted_cueing\adapted_cueing_v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L\Root\projects\visual-working-memory\protocol\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F166716-1846-4B0B-885A-8548E7E24FAA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B653029C-2893-4C4D-8760-BD11A3767046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{18036FE8-5AE1-4DFA-B28E-FC5D77AF1D80}"/>
   </bookViews>
@@ -23,7 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>load</t>
   </si>
@@ -187,6 +191,27 @@
   </si>
   <si>
     <t>practice</t>
+  </si>
+  <si>
+    <t>[-0.843137254901961, -0.929411764705882, 0.568627450980392]</t>
+  </si>
+  <si>
+    <t>[0.984313725490196, 0.992156862745098, -0.835294117647059]</t>
+  </si>
+  <si>
+    <t>[-1, 0.96078431372549, -0.976470588235294]</t>
+  </si>
+  <si>
+    <t>[-0.843137254901961, 0.984313725490196, 1]</t>
+  </si>
+  <si>
+    <t>[0.888, 0.888, 0.888]</t>
+  </si>
+  <si>
+    <t>[1, -0.67843137254902, 1]</t>
+  </si>
+  <si>
+    <t>[-0.23922, -0.41176, -0.34902]</t>
   </si>
 </sst>
 </file>
@@ -555,11 +580,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826EEF42-B807-46DB-92AD-A8D47120DC3D}">
   <dimension ref="A1:AQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AP4" sqref="AP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="32" max="32" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="57.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="40" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="55.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -798,53 +833,41 @@
         <f t="shared" si="1"/>
         <v>X</v>
       </c>
-      <c r="AF2" t="str">
-        <f>_xlfn.IFS(T2="RED","red",T2="GREEN","limegreen",T2="BLUE","dodgerblue",T2="CYAN","aqua",T2="YELLOW","yellow",T2="WHITE","white",T2="PURPLE","magenta",T2="X","black")</f>
-        <v>dodgerblue</v>
-      </c>
-      <c r="AG2" t="str">
-        <f t="shared" ref="AG2:AQ4" si="2">_xlfn.IFS(U2="RED","red",U2="GREEN","limegreen",U2="BLUE","dodgerblue",U2="CYAN","aqua",U2="YELLOW","yellow",U2="WHITE","white",U2="PURPLE","magenta",U2="X","black")</f>
-        <v>black</v>
-      </c>
-      <c r="AH2" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AI2" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AJ2" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AK2" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AL2" t="str">
-        <f t="shared" si="2"/>
-        <v>dodgerblue</v>
-      </c>
-      <c r="AM2" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AN2" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AO2" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AP2" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AQ2" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
+      <c r="AF2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:43" x14ac:dyDescent="0.25">
@@ -906,100 +929,88 @@
         <v>34</v>
       </c>
       <c r="T3" t="str">
-        <f t="shared" ref="T3:Y4" si="3">IF(E3=1,M3,"X")</f>
+        <f t="shared" ref="T3:Y4" si="2">IF(E3=1,M3,"X")</f>
         <v>X</v>
       </c>
       <c r="U3" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="V3" t="str">
+        <f t="shared" si="2"/>
+        <v>CYAN</v>
+      </c>
+      <c r="W3" t="str">
+        <f t="shared" si="2"/>
+        <v>YELLOW</v>
+      </c>
+      <c r="X3" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="Y3" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="Z3" t="str">
+        <f t="shared" ref="Z3:AE4" si="3">IF($K3=0,T3,IF(T3=INDEX($T3:$Y3,1,$L3),$S3,T3))</f>
+        <v>X</v>
+      </c>
+      <c r="AA3" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="V3" t="str">
+      <c r="AB3" t="str">
         <f t="shared" si="3"/>
-        <v>CYAN</v>
-      </c>
-      <c r="W3" t="str">
+        <v>GREEN</v>
+      </c>
+      <c r="AC3" t="str">
         <f t="shared" si="3"/>
         <v>YELLOW</v>
       </c>
-      <c r="X3" t="str">
+      <c r="AD3" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="Y3" t="str">
+      <c r="AE3" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="Z3" t="str">
-        <f t="shared" ref="Z3:AE4" si="4">IF($K3=0,T3,IF(T3=INDEX($T3:$Y3,1,$L3),$S3,T3))</f>
-        <v>X</v>
-      </c>
-      <c r="AA3" t="str">
-        <f t="shared" si="4"/>
-        <v>X</v>
-      </c>
-      <c r="AB3" t="str">
-        <f t="shared" si="4"/>
-        <v>GREEN</v>
-      </c>
-      <c r="AC3" t="str">
-        <f t="shared" si="4"/>
-        <v>YELLOW</v>
-      </c>
-      <c r="AD3" t="str">
-        <f t="shared" si="4"/>
-        <v>X</v>
-      </c>
-      <c r="AE3" t="str">
-        <f t="shared" si="4"/>
-        <v>X</v>
-      </c>
-      <c r="AF3" t="str">
-        <f t="shared" ref="AF3:AF4" si="5">_xlfn.IFS(T3="RED","red",T3="GREEN","limegreen",T3="BLUE","dodgerblue",T3="CYAN","aqua",T3="YELLOW","yellow",T3="WHITE","white",T3="PURPLE","magenta",T3="X","black")</f>
-        <v>black</v>
-      </c>
-      <c r="AG3" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AH3" t="str">
-        <f t="shared" si="2"/>
-        <v>aqua</v>
-      </c>
-      <c r="AI3" t="str">
-        <f t="shared" si="2"/>
-        <v>yellow</v>
-      </c>
-      <c r="AJ3" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AK3" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AL3" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AM3" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AN3" t="str">
-        <f t="shared" si="2"/>
-        <v>limegreen</v>
-      </c>
-      <c r="AO3" t="str">
-        <f t="shared" si="2"/>
-        <v>yellow</v>
-      </c>
-      <c r="AP3" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AQ3" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
+      <c r="AF3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AO3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:43" x14ac:dyDescent="0.25">
@@ -1061,100 +1072,88 @@
         <v>36</v>
       </c>
       <c r="T4" t="str">
+        <f t="shared" si="2"/>
+        <v>YELLOW</v>
+      </c>
+      <c r="U4" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="V4" t="str">
+        <f t="shared" si="2"/>
+        <v>WHITE</v>
+      </c>
+      <c r="W4" t="str">
+        <f t="shared" si="2"/>
+        <v>GREEN</v>
+      </c>
+      <c r="X4" t="str">
+        <f t="shared" si="2"/>
+        <v>X</v>
+      </c>
+      <c r="Y4" t="str">
+        <f t="shared" si="2"/>
+        <v>PURPLE</v>
+      </c>
+      <c r="Z4" t="str">
         <f t="shared" si="3"/>
         <v>YELLOW</v>
       </c>
-      <c r="U4" t="str">
+      <c r="AA4" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="V4" t="str">
+      <c r="AB4" t="str">
         <f t="shared" si="3"/>
-        <v>WHITE</v>
-      </c>
-      <c r="W4" t="str">
+        <v>CYAN</v>
+      </c>
+      <c r="AC4" t="str">
         <f t="shared" si="3"/>
         <v>GREEN</v>
       </c>
-      <c r="X4" t="str">
+      <c r="AD4" t="str">
         <f t="shared" si="3"/>
         <v>X</v>
       </c>
-      <c r="Y4" t="str">
+      <c r="AE4" t="str">
         <f t="shared" si="3"/>
         <v>PURPLE</v>
       </c>
-      <c r="Z4" t="str">
-        <f t="shared" si="4"/>
-        <v>YELLOW</v>
-      </c>
-      <c r="AA4" t="str">
-        <f t="shared" si="4"/>
-        <v>X</v>
-      </c>
-      <c r="AB4" t="str">
-        <f t="shared" si="4"/>
-        <v>CYAN</v>
-      </c>
-      <c r="AC4" t="str">
-        <f t="shared" si="4"/>
-        <v>GREEN</v>
-      </c>
-      <c r="AD4" t="str">
-        <f t="shared" si="4"/>
-        <v>X</v>
-      </c>
-      <c r="AE4" t="str">
-        <f t="shared" si="4"/>
-        <v>PURPLE</v>
-      </c>
-      <c r="AF4" t="str">
-        <f t="shared" si="5"/>
-        <v>yellow</v>
-      </c>
-      <c r="AG4" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AH4" t="str">
-        <f t="shared" si="2"/>
-        <v>white</v>
-      </c>
-      <c r="AI4" t="str">
-        <f t="shared" si="2"/>
-        <v>limegreen</v>
-      </c>
-      <c r="AJ4" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AK4" t="str">
-        <f t="shared" si="2"/>
-        <v>magenta</v>
-      </c>
-      <c r="AL4" t="str">
-        <f t="shared" si="2"/>
-        <v>yellow</v>
-      </c>
-      <c r="AM4" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AN4" t="str">
-        <f t="shared" si="2"/>
-        <v>aqua</v>
-      </c>
-      <c r="AO4" t="str">
-        <f t="shared" si="2"/>
-        <v>limegreen</v>
-      </c>
-      <c r="AP4" t="str">
-        <f t="shared" si="2"/>
-        <v>black</v>
-      </c>
-      <c r="AQ4" t="str">
-        <f t="shared" si="2"/>
-        <v>magenta</v>
+      <c r="AF4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AP4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>